<commit_message>
enhance data retrieval and processing; save results to Reliance.xlsx
</commit_message>
<xml_diff>
--- a/Reliance.xlsx
+++ b/Reliance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1415,6 +1415,916 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-10-31 09:15:00</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>302500</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2259000</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-10-31 09:45:00</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>124000</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2176000</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-10-31 10:15:00</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>21000</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2169000</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-10-31 10:45:00</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>24500</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2157500</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-10-31 11:15:00</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>12500</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2133500</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-10-31 11:45:00</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2132000</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-10-31 12:15:00</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>13000</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2133000</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-10-31 12:45:00</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2133000</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-10-31 13:15:00</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2133500</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-10-31 13:45:00</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>17000</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2120500</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-10-31 14:15:00</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2099000</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-10-31 14:45:00</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>2079000</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-10-31 15:15:00</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>RELIND</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Options</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>31-OCT-24</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>.05</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>2076000</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor date handling and parameters
</commit_message>
<xml_diff>
--- a/Reliance.xlsx
+++ b/Reliance.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -543,32 +543,32 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>14.5</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>18.6</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>30.1</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>30.75</t>
+          <t>10.55</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>14500</t>
+          <t>319200</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>202000</t>
+          <t>822500</t>
         </is>
       </c>
       <c r="N2" t="n">
@@ -583,7 +583,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -613,32 +613,32 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>31.7</t>
+          <t>11.75</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>36.35</t>
+          <t>15.55</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>31.7</t>
+          <t>11.75</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>34.5</t>
+          <t>11.95</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>10000</t>
+          <t>98700</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>194000</t>
+          <t>790300</t>
         </is>
       </c>
       <c r="N3" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -683,32 +683,32 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>35.85</t>
+          <t>11.4</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>37.8</t>
+          <t>11.75</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>35.85</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>37.45</t>
+          <t>9.95</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>76300</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>191000</t>
+          <t>774900</t>
         </is>
       </c>
       <c r="N4" t="n">
@@ -723,7 +723,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -753,32 +753,32 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>37.35</t>
+          <t>9.25</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>37.35</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>35.65</t>
+          <t>7.55</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>36.15</t>
+          <t>8.15</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>109200</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>190500</t>
+          <t>737100</t>
         </is>
       </c>
       <c r="N5" t="n">
@@ -793,7 +793,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -823,32 +823,32 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>34.35</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>34.35</t>
+          <t>8.85</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>32.95</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>34.25</t>
+          <t>7.15</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>567700</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>183500</t>
+          <t>868700</t>
         </is>
       </c>
       <c r="N6" t="n">
@@ -863,7 +863,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -893,32 +893,32 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>34.65</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>34.65</t>
+          <t>5.25</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>5.95</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>115500</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>182000</t>
+          <t>875700</t>
         </is>
       </c>
       <c r="N7" t="n">
@@ -933,7 +933,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -963,32 +963,32 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>37.8</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>39.1</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>37.5</t>
+          <t>2.65</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>428400</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>184000</t>
+          <t>877100</t>
         </is>
       </c>
       <c r="N8" t="n">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1033,32 +1033,32 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>37.2</t>
+          <t>2.85</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>37.2</t>
+          <t>2.45</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>38.85</t>
+          <t>4.75</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>6000</t>
+          <t>211400</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>177500</t>
+          <t>838600</t>
         </is>
       </c>
       <c r="N9" t="n">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1103,32 +1103,32 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>4.95</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>32.25</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>37.35</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>8000</t>
+          <t>133700</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>172500</t>
+          <t>838600</t>
         </is>
       </c>
       <c r="N10" t="n">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1173,32 +1173,32 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>36.55</t>
+          <t>5.45</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>37.85</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>32.8</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>32.8</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>23500</t>
+          <t>347900</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>169500</t>
+          <t>824600</t>
         </is>
       </c>
       <c r="N11" t="n">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1243,32 +1243,32 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>32.5</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>32.5</t>
+          <t>1.35</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>26.15</t>
+          <t>.05</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>29.15</t>
+          <t>.1</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>9000</t>
+          <t>673400</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>166500</t>
+          <t>870800</t>
         </is>
       </c>
       <c r="N12" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1313,32 +1313,32 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>28.6</t>
+          <t>.15</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>.35</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>27.5</t>
+          <t>.05</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>29.55</t>
+          <t>.05</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>13000</t>
+          <t>256900</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>165500</t>
+          <t>786800</t>
         </is>
       </c>
       <c r="N13" t="n">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1383,32 +1383,32 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>31.5</t>
+          <t>.2</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>31.7</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>29.05</t>
+          <t>.05</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>29.05</t>
+          <t>.05</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>5500</t>
+          <t>153300</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>164000</t>
+          <t>770000</t>
         </is>
       </c>
       <c r="N14" t="n">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1453,32 +1453,32 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>.1</t>
+          <t>.85</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>.1</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>.6</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.75</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>302500</t>
+          <t>579600</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2259000</t>
+          <t>1472800</t>
         </is>
       </c>
       <c r="N15" t="n">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1523,32 +1523,32 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>.1</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>.1</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>.85</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>.1</t>
+          <t>1.15</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>124000</t>
+          <t>122500</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2176000</t>
+          <t>1428700</t>
         </is>
       </c>
       <c r="N16" t="n">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1593,32 +1593,32 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>.75</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>21000</t>
+          <t>196000</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2169000</t>
+          <t>1385300</t>
         </is>
       </c>
       <c r="N17" t="n">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1663,32 +1663,32 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.15</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.45</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>24500</t>
+          <t>203700</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2157500</t>
+          <t>1334900</t>
         </is>
       </c>
       <c r="N18" t="n">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1733,32 +1733,32 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.45</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>.95</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>12500</t>
+          <t>710500</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2133500</t>
+          <t>1360100</t>
         </is>
       </c>
       <c r="N19" t="n">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1803,32 +1803,32 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.7</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>237300</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2132000</t>
+          <t>1311800</t>
         </is>
       </c>
       <c r="N20" t="n">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1873,32 +1873,32 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.55</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.35</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>13000</t>
+          <t>628600</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2133000</t>
+          <t>1092000</t>
         </is>
       </c>
       <c r="N21" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1943,32 +1943,32 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.65</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>397600</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2133000</t>
+          <t>979300</t>
         </is>
       </c>
       <c r="N22" t="n">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2013,32 +2013,32 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.65</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>6000</t>
+          <t>176400</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2133500</t>
+          <t>997500</t>
         </is>
       </c>
       <c r="N23" t="n">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2083,32 +2083,32 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.05</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>.85</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.05</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>17000</t>
+          <t>253400</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2120500</t>
+          <t>984900</t>
         </is>
       </c>
       <c r="N24" t="n">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2153,32 +2153,32 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.15</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>3.15</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>8.15</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>50000</t>
+          <t>419300</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>2099000</t>
+          <t>866600</t>
         </is>
       </c>
       <c r="N25" t="n">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2223,32 +2223,32 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>292600</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2079000</t>
+          <t>686000</t>
         </is>
       </c>
       <c r="N26" t="n">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>RELIND</t>
+          <t>ICIBAN</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2293,32 +2293,32 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>.05</t>
+          <t>4</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>156800</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>2076000</t>
+          <t>638400</t>
         </is>
       </c>
       <c r="N27" t="n">

</xml_diff>